<commit_message>
Improved analog circuit design for AD9286 and AD9239
</commit_message>
<xml_diff>
--- a/documents/其他ADDA的分析.xlsx
+++ b/documents/其他ADDA的分析.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AD9286 - Plan A" sheetId="1" r:id="rId1"/>
+    <sheet name="AD9286 - Plan B" sheetId="2" r:id="rId2"/>
+    <sheet name="AD9239 - Plan A" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,15 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
-    <t>Vo(low freq)</t>
+    <t>offset</t>
   </si>
   <si>
-    <t>Vo(500Hz)</t>
+    <t>Vo/V(low freq)</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1/Ω</t>
+  </si>
+  <si>
+    <t>Vo/V(500MHz)</t>
+  </si>
+  <si>
+    <t>Vo/V(250MHz)</t>
   </si>
 </sst>
 </file>
@@ -57,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,12 +73,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -387,186 +412,837 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>200</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>33.869999999999997</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>38.515999999999998</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f>(C2-B2)/B2</f>
         <v>0.13717153823442577</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>220</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>37.213000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>42.930999999999997</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D12" si="0">(C3-B3)/B3</f>
         <v>0.15365598043694398</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>240</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>40.548000000000002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>47.466999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>0.17063726940909532</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>260</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>43.875999999999998</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>52.128</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>0.18807548545902095</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>280</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>47.195999999999998</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>56.920999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>0.20605559793202818</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>300</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>50.508000000000003</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>61.851999999999997</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>0.22459808347192511</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>320</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>53.813000000000002</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>66.926000000000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0.24367717837697209</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>340</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>57.11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>72.150000000000006</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0.26335142707056569</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>360</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>60.399000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>77.533000000000001</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0.28368019338068512</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>380</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>63.68</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>83.08</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f>(C11-B11)/B11</f>
         <v>0.30464824120603012</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>400</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>66.953999999999994</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>88.8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.32628371717895877</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>200</v>
+      </c>
+      <c r="B2" s="1">
+        <v>33.869999999999997</v>
+      </c>
+      <c r="C2" s="1">
+        <v>34.938000000000002</v>
+      </c>
+      <c r="D2" s="2">
+        <f>(C2-B2)/B2</f>
+        <v>3.1532329495128582E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>250</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42.213000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43.905999999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D22" si="0">(C3-B3)/B3</f>
+        <v>4.0106128443844265E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>300</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50.508000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>52.973999999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8823948681396882E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>350</v>
+      </c>
+      <c r="B5" s="1">
+        <v>58.755000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <v>62.143000000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>5.7663177601906188E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>400</v>
+      </c>
+      <c r="B6" s="1">
+        <v>66.953999999999994</v>
+      </c>
+      <c r="C6" s="1">
+        <v>71.417000000000002</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>6.6657705290199362E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>450</v>
+      </c>
+      <c r="B7" s="1">
+        <v>75.105999999999995</v>
+      </c>
+      <c r="C7" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>7.5812851170345946E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>500</v>
+      </c>
+      <c r="B8" s="1">
+        <v>83.21</v>
+      </c>
+      <c r="C8" s="1">
+        <v>90.293999999999997</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5133998317509965E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>550</v>
+      </c>
+      <c r="B9" s="1">
+        <v>91.269000000000005</v>
+      </c>
+      <c r="C9" s="1">
+        <v>99.903000000000006</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4599480656082563E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>600</v>
+      </c>
+      <c r="B10" s="1">
+        <v>99.28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>109.63</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10425060435132952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>650</v>
+      </c>
+      <c r="B11" s="1">
+        <v>107.247</v>
+      </c>
+      <c r="C11" s="1">
+        <v>119.47799999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11404514811603117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>700</v>
+      </c>
+      <c r="B12" s="1">
+        <v>115.16800000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>129.453</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12403619060850232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>750</v>
+      </c>
+      <c r="B13" s="1">
+        <v>123.04300000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>139.55600000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13420511528490042</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>800</v>
+      </c>
+      <c r="B14" s="1">
+        <v>130.875</v>
+      </c>
+      <c r="C14" s="1">
+        <v>149.79300000000001</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14455014326647569</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>850</v>
+      </c>
+      <c r="B15" s="1">
+        <v>138.66200000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>160.167</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15508935396864312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>900</v>
+      </c>
+      <c r="B16" s="1">
+        <v>146.405</v>
+      </c>
+      <c r="C16" s="1">
+        <v>170.68299999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16582766982001976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>950</v>
+      </c>
+      <c r="B17" s="1">
+        <v>154.10499999999999</v>
+      </c>
+      <c r="C17" s="1">
+        <v>181.345</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17676259693066423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>161.762</v>
+      </c>
+      <c r="C18" s="1">
+        <v>192.15799999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18790568860424567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>1050</v>
+      </c>
+      <c r="B19" s="1">
+        <v>169.376</v>
+      </c>
+      <c r="C19" s="1">
+        <v>203.126</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19926081617230304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>1100</v>
+      </c>
+      <c r="B20" s="1">
+        <v>176.947</v>
+      </c>
+      <c r="C20" s="1">
+        <v>214.25399999999999</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21083714332540246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>1150</v>
+      </c>
+      <c r="B21" s="1">
+        <v>184.477</v>
+      </c>
+      <c r="C21" s="1">
+        <v>225.547</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22262937927221274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>1200</v>
+      </c>
+      <c r="B22" s="1">
+        <v>191.965</v>
+      </c>
+      <c r="C22" s="1">
+        <v>237.011</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23465735941447655</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>200</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.4217999999999993</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8.4868000000000006</v>
+      </c>
+      <c r="D2" s="1">
+        <f>(C2-B2)/B2</f>
+        <v>7.7180650217294738E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>450</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18.687000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>19.023</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D18" si="0">(C3-B3)/B3</f>
+        <v>1.7980414191683978E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>700</v>
+      </c>
+      <c r="B4" s="1">
+        <v>28.672999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29.489000000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8458828863390736E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>950</v>
+      </c>
+      <c r="B5" s="1">
+        <v>38.390999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>39.892000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9097705191321011E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>1200</v>
+      </c>
+      <c r="B6" s="1">
+        <v>47.85</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50.244</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0031347962382407E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>1450</v>
+      </c>
+      <c r="B7" s="1">
+        <v>57.061999999999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>60.552</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.116154358417164E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>1700</v>
+      </c>
+      <c r="B8" s="1">
+        <v>66.036000000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70.825999999999993</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2536192379913864E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>1950</v>
+      </c>
+      <c r="B9" s="1">
+        <v>74.781000000000006</v>
+      </c>
+      <c r="C9" s="1">
+        <v>81.073999999999998</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4152391650285388E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>2200</v>
+      </c>
+      <c r="B10" s="1">
+        <v>83.305999999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>91.305999999999997</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6031498331452719E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>2450</v>
+      </c>
+      <c r="B11" s="1">
+        <v>91.617999999999995</v>
+      </c>
+      <c r="C11" s="1">
+        <v>101.53</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10818834726800418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>2700</v>
+      </c>
+      <c r="B12" s="1">
+        <v>99.727000000000004</v>
+      </c>
+      <c r="C12" s="1">
+        <v>111.754</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.12059923591404535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>2950</v>
+      </c>
+      <c r="B13" s="1">
+        <v>107.63800000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>121.986</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13329864917594156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>3200</v>
+      </c>
+      <c r="B14" s="1">
+        <v>115.36</v>
+      </c>
+      <c r="C14" s="1">
+        <v>132.23599999999999</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14628987517337025</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>3450</v>
+      </c>
+      <c r="B15" s="1">
+        <v>122.899</v>
+      </c>
+      <c r="C15" s="1">
+        <v>142.512</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.15958632698394618</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>3700</v>
+      </c>
+      <c r="B16" s="1">
+        <v>130.262</v>
+      </c>
+      <c r="C16" s="1">
+        <v>152.822</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17318941824937437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>3950</v>
+      </c>
+      <c r="B17" s="1">
+        <v>137.45400000000001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>163.17500000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.18712441980589872</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>4200</v>
+      </c>
+      <c r="B18" s="1">
+        <v>144.482</v>
+      </c>
+      <c r="C18" s="1">
+        <v>173.58</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20139532952201666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simulation of single-end voltages added
</commit_message>
<xml_diff>
--- a/documents/其他ADDA的分析.xlsx
+++ b/documents/其他ADDA的分析.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AD9286 - Plan A" sheetId="1" r:id="rId1"/>
     <sheet name="AD9286 - Plan B" sheetId="2" r:id="rId2"/>
     <sheet name="AD9239 - Plan A" sheetId="3" r:id="rId3"/>
+    <sheet name="Error Analysis" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -92,10 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -964,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
@@ -1248,4 +1250,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1">
+        <v>-3.6051000000000002</v>
+      </c>
+      <c r="B1">
+        <v>1.6926000000000001</v>
+      </c>
+      <c r="C1">
+        <f>1.4-A1/12</f>
+        <v>1.7004249999999999</v>
+      </c>
+      <c r="D1">
+        <f>B1-C1</f>
+        <v>-7.8249999999997488E-3</v>
+      </c>
+      <c r="E1" s="3">
+        <f>D1 / C1</f>
+        <v>-4.6017907287882439E-3</v>
+      </c>
+      <c r="F1">
+        <v>1.0886</v>
+      </c>
+      <c r="G1">
+        <f>1.4+A1/12</f>
+        <v>1.099575</v>
+      </c>
+      <c r="H1">
+        <f>F1-G1</f>
+        <v>-1.0974999999999957E-2</v>
+      </c>
+      <c r="I1" s="3">
+        <f>H1 / G1</f>
+        <v>-9.9811290725961913E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>3.5987</v>
+      </c>
+      <c r="B2">
+        <v>1.1024</v>
+      </c>
+      <c r="C2">
+        <f>1.4-A2/12</f>
+        <v>1.1001083333333332</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>2.2916666666668029E-3</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2 / C2</f>
+        <v>2.0831281767705935E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.6997</v>
+      </c>
+      <c r="G2">
+        <f>1.4+A2/12</f>
+        <v>1.6998916666666666</v>
+      </c>
+      <c r="H2">
+        <f>F2-G2</f>
+        <v>-1.9166666666659005E-4</v>
+      </c>
+      <c r="I2" s="3">
+        <f>H2 / G2</f>
+        <v>-1.1275228323369041E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>